<commit_message>
Vogeltje is af en geprefabt
Vogeltje is done en heb wat meer bugs tegevoegd
</commit_message>
<xml_diff>
--- a/Algemeen/Bug Reports/Bug Report.xlsx
+++ b/Algemeen/Bug Reports/Bug Report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>Bug nr.</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Door de pistol een child van een extra gameobject</t>
   </si>
   <si>
-    <t>Dev-Fase-</t>
-  </si>
-  <si>
     <t>Dev-Fase-2</t>
   </si>
   <si>
@@ -188,6 +185,102 @@
   </si>
   <si>
     <t>de originele hoogte</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>De White-out werkt soms niet wanneer je een</t>
+  </si>
+  <si>
+    <t>nieuw spel start.</t>
+  </si>
+  <si>
+    <t>Dat het altijd werkt</t>
+  </si>
+  <si>
+    <t>Het werkt dus niet altijd</t>
+  </si>
+  <si>
+    <t>Stap 1: Start spel op en druk op start</t>
+  </si>
+  <si>
+    <t>Stap2: Let wel op dat het alleen soms niet blijkt te werken.</t>
+  </si>
+  <si>
+    <t>Stap 3: ???</t>
+  </si>
+  <si>
+    <t>Stap 4: Profit?</t>
+  </si>
+  <si>
+    <t>Moet nog opgelost worden.</t>
+  </si>
+  <si>
+    <t>Ma&amp;Fa</t>
+  </si>
+  <si>
+    <t>De turret gaat negeert de speler nadat hij de speler</t>
+  </si>
+  <si>
+    <t>voor de tweede keer ziet.</t>
+  </si>
+  <si>
+    <t>Dat de turret de speler nooit negeert</t>
+  </si>
+  <si>
+    <t>De turret negeert de speler na de eerste keer</t>
+  </si>
+  <si>
+    <t>Stap 1: Tijdens het spelen laat je de turret je zien</t>
+  </si>
+  <si>
+    <t>Stap 2: Verlaat de zicht van de turret</t>
+  </si>
+  <si>
+    <t>Stap 3: Keer terug en wordt genegeerd door de turret</t>
+  </si>
+  <si>
+    <t>Stap 4: Je bent de profit gewoon niet waard</t>
+  </si>
+  <si>
+    <t>De x van de rotation moest terug gezet worden naar wat</t>
+  </si>
+  <si>
+    <t>het was bij zijn start. Hij veranderde de x as nadat de speler</t>
+  </si>
+  <si>
+    <t>weg ging.</t>
+  </si>
+  <si>
+    <t>Kunt tijdens de intro het spel pauzeren.</t>
+  </si>
+  <si>
+    <t>Dat je niet kunt pauzeren tijdens de intro</t>
+  </si>
+  <si>
+    <t>Je kunt dus wel pauzeren tijdens de intro</t>
+  </si>
+  <si>
+    <t>Stap 1: Start het spel</t>
+  </si>
+  <si>
+    <t>Stap 2: Druk escape tijden de intro</t>
+  </si>
+  <si>
+    <t>Stap 3: Zie dat het spel inderdaad pauzeerd</t>
+  </si>
+  <si>
+    <t>Stap 4: Geniet van de profit!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fahretin heeft een boolerino toegevoegd, "mayPause" </t>
+  </si>
+  <si>
+    <t>zodat hij pas na de intro kan.</t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -720,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L60"/>
+  <dimension ref="A1:L88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1115,7 @@
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="18">
@@ -1034,11 +1127,11 @@
       </c>
       <c r="I21" s="18"/>
       <c r="J21" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K21" s="18"/>
       <c r="L21" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1060,14 +1153,14 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
       <c r="F23" s="24"/>
       <c r="G23" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -1077,14 +1170,14 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="6"/>
       <c r="G24" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -1099,7 +1192,7 @@
       <c r="E25" s="12"/>
       <c r="F25" s="6"/>
       <c r="G25" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -1114,7 +1207,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="6"/>
       <c r="G26" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -1141,14 +1234,14 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
       <c r="F28" s="6"/>
       <c r="G28" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -1165,7 +1258,7 @@
       <c r="E29" s="12"/>
       <c r="F29" s="6"/>
       <c r="G29" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -1175,7 +1268,7 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -1212,13 +1305,13 @@
         <v>23</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>25</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H32" s="31"/>
       <c r="I32" s="31"/>
@@ -1258,7 +1351,7 @@
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E35" s="18"/>
       <c r="F35" s="18">
@@ -1270,7 +1363,7 @@
       </c>
       <c r="I35" s="18"/>
       <c r="J35" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K35" s="18"/>
       <c r="L35" s="19" t="s">
@@ -1296,14 +1389,14 @@
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="23"/>
       <c r="E37" s="23"/>
       <c r="F37" s="24"/>
       <c r="G37" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H37" s="23"/>
       <c r="I37" s="23"/>
@@ -1313,14 +1406,14 @@
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="6"/>
       <c r="G38" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H38" s="12"/>
       <c r="I38" s="12"/>
@@ -1335,7 +1428,7 @@
       <c r="E39" s="12"/>
       <c r="F39" s="6"/>
       <c r="G39" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
@@ -1350,7 +1443,7 @@
       <c r="E40" s="12"/>
       <c r="F40" s="6"/>
       <c r="G40" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
@@ -1377,14 +1470,14 @@
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="6"/>
       <c r="G42" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
@@ -1401,7 +1494,7 @@
       <c r="E43" s="12"/>
       <c r="F43" s="6"/>
       <c r="G43" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
@@ -1411,7 +1504,7 @@
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -1426,7 +1519,7 @@
     </row>
     <row r="45" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1450,7 +1543,7 @@
         <v>23</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>25</v>
@@ -1490,7 +1583,7 @@
     </row>
     <row r="49" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18" t="s">
@@ -1498,16 +1591,20 @@
       </c>
       <c r="E49" s="18"/>
       <c r="F49" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="18"/>
       <c r="H49" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
+      <c r="J49" s="18" t="s">
+        <v>57</v>
+      </c>
       <c r="K49" s="18"/>
-      <c r="L49" s="19"/>
+      <c r="L49" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="50" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="26" t="s">
@@ -1527,12 +1624,16 @@
       <c r="L50" s="30"/>
     </row>
     <row r="51" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B51" s="22"/>
+      <c r="B51" s="22" t="s">
+        <v>58</v>
+      </c>
       <c r="C51" s="23"/>
       <c r="D51" s="23"/>
       <c r="E51" s="23"/>
       <c r="F51" s="24"/>
-      <c r="G51" s="22"/>
+      <c r="G51" s="22" t="s">
+        <v>62</v>
+      </c>
       <c r="H51" s="23"/>
       <c r="I51" s="23"/>
       <c r="J51" s="23"/>
@@ -1540,12 +1641,16 @@
       <c r="L51" s="24"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
+      <c r="B52" s="20" t="s">
+        <v>59</v>
+      </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
       <c r="F52" s="6"/>
-      <c r="G52" s="20"/>
+      <c r="G52" s="20" t="s">
+        <v>63</v>
+      </c>
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
@@ -1558,7 +1663,9 @@
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
       <c r="F53" s="6"/>
-      <c r="G53" s="20"/>
+      <c r="G53" s="20" t="s">
+        <v>64</v>
+      </c>
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
@@ -1571,7 +1678,9 @@
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="20"/>
+      <c r="G54" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
@@ -1596,12 +1705,16 @@
       <c r="L55" s="6"/>
     </row>
     <row r="56" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B56" s="20"/>
+      <c r="B56" s="20" t="s">
+        <v>60</v>
+      </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
       <c r="F56" s="6"/>
-      <c r="G56" s="20"/>
+      <c r="G56" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
@@ -1624,7 +1737,9 @@
       <c r="L57" s="6"/>
     </row>
     <row r="58" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B58" s="20"/>
+      <c r="B58" s="20" t="s">
+        <v>61</v>
+      </c>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
@@ -1653,11 +1768,15 @@
       <c r="B60" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D60" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="F60" s="3" t="s">
         <v>25</v>
       </c>
@@ -1668,6 +1787,478 @@
       <c r="K60" s="31"/>
       <c r="L60" s="31"/>
     </row>
+    <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="27"/>
+      <c r="D62" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="27"/>
+      <c r="F62" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" s="27"/>
+      <c r="H62" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I62" s="27"/>
+      <c r="J62" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" s="27"/>
+      <c r="L62" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="17">
+        <v>5</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18">
+        <v>4</v>
+      </c>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18">
+        <v>2</v>
+      </c>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K63" s="18"/>
+      <c r="L63" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="27"/>
+      <c r="F64" s="27"/>
+      <c r="G64" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H64" s="27"/>
+      <c r="I64" s="27"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="27"/>
+      <c r="L64" s="30"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B65" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" s="23"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="23"/>
+      <c r="F65" s="24"/>
+      <c r="G65" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H65" s="23"/>
+      <c r="I65" s="23"/>
+      <c r="J65" s="23"/>
+      <c r="K65" s="23"/>
+      <c r="L65" s="24"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B66" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+      <c r="L66" s="6"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B67" s="20"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+      <c r="L67" s="6"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B68" s="20"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+      <c r="L68" s="6"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B69" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+      <c r="L69" s="6"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B70" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+      <c r="L70" s="6"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B71" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+      <c r="L71" s="6"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+      <c r="L72" s="6"/>
+    </row>
+    <row r="73" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="21"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="8"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7"/>
+      <c r="K73" s="7"/>
+      <c r="L73" s="8"/>
+    </row>
+    <row r="74" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H74" s="31"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="31"/>
+      <c r="K74" s="31"/>
+      <c r="L74" s="31"/>
+    </row>
+    <row r="75" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C76" s="27"/>
+      <c r="D76" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" s="27"/>
+      <c r="F76" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G76" s="27"/>
+      <c r="H76" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I76" s="27"/>
+      <c r="J76" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="K76" s="27"/>
+      <c r="L76" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="17">
+        <v>6</v>
+      </c>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E77" s="18"/>
+      <c r="F77" s="18">
+        <v>1</v>
+      </c>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18">
+        <v>1</v>
+      </c>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K77" s="18"/>
+      <c r="L77" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="27"/>
+      <c r="F78" s="27"/>
+      <c r="G78" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="H78" s="27"/>
+      <c r="I78" s="27"/>
+      <c r="J78" s="27"/>
+      <c r="K78" s="27"/>
+      <c r="L78" s="30"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="23"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="23"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="H79" s="23"/>
+      <c r="I79" s="23"/>
+      <c r="J79" s="23"/>
+      <c r="K79" s="23"/>
+      <c r="L79" s="24"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B80" s="20"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+      <c r="L80" s="6"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B81" s="20"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+      <c r="L81" s="6"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B82" s="20"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+      <c r="L82" s="6"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+      <c r="L83" s="6"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B84" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+      <c r="L84" s="6"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="13"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+      <c r="L85" s="6"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B86" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+      <c r="L86" s="6"/>
+    </row>
+    <row r="87" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="21"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="8"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="7"/>
+      <c r="I87" s="7"/>
+      <c r="J87" s="7"/>
+      <c r="K87" s="7"/>
+      <c r="L87" s="8"/>
+    </row>
+    <row r="88" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" s="31"/>
+      <c r="I88" s="31"/>
+      <c r="J88" s="31"/>
+      <c r="K88" s="31"/>
+      <c r="L88" s="31"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>